<commit_message>
visiting_card design 49.avif changes done
</commit_message>
<xml_diff>
--- a/Visiting Card - User Assignment Mapping.xlsx
+++ b/Visiting Card - User Assignment Mapping.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27726"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21629"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Ketan Mali\OneDrive - Apnasite IT Services Private Limited\Desktop\Git Repo\visiting-card-assignments\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\New_Ass\visiting-card-assignments\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4FE83554-25E0-4FCE-8226-2E0D38C6AFF6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{74EAEB26-8797-4625-984C-927EF696984C}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -23,12 +23,6 @@
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
         <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
-        <xcalcf:feature name="microsoft.com:LET_WF"/>
-        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
-        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -974,19 +968,19 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:F155"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+    <sheetView tabSelected="1" topLeftCell="A48" workbookViewId="0">
+      <selection activeCell="B50" sqref="B50"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="28.7265625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="11.7265625" customWidth="1"/>
-    <col min="4" max="4" width="19.453125" customWidth="1"/>
-    <col min="5" max="5" width="24.26953125" customWidth="1"/>
+    <col min="2" max="2" width="28.7109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.7109375" customWidth="1"/>
+    <col min="4" max="4" width="19.42578125" customWidth="1"/>
+    <col min="5" max="5" width="24.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1006,7 +1000,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="2" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2">
         <v>1</v>
       </c>
@@ -1022,7 +1016,7 @@
       </c>
       <c r="F2" s="26"/>
     </row>
-    <row r="3" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="3" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A3">
         <v>2</v>
       </c>
@@ -1038,7 +1032,7 @@
       </c>
       <c r="F3" s="26"/>
     </row>
-    <row r="4" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="4" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A4">
         <v>3</v>
       </c>
@@ -1054,7 +1048,7 @@
       </c>
       <c r="F4" s="26"/>
     </row>
-    <row r="5" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="5" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A5">
         <v>4</v>
       </c>
@@ -1070,7 +1064,7 @@
       </c>
       <c r="F5" s="26"/>
     </row>
-    <row r="6" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="6" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A6">
         <v>5</v>
       </c>
@@ -1086,7 +1080,7 @@
       </c>
       <c r="F6" s="26"/>
     </row>
-    <row r="7" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="7" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A7">
         <v>6</v>
       </c>
@@ -1102,7 +1096,7 @@
       </c>
       <c r="F7" s="26"/>
     </row>
-    <row r="8" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="8" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A8">
         <v>7</v>
       </c>
@@ -1118,7 +1112,7 @@
       </c>
       <c r="F8" s="26"/>
     </row>
-    <row r="9" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="9" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A9">
         <v>8</v>
       </c>
@@ -1134,7 +1128,7 @@
       </c>
       <c r="F9" s="26"/>
     </row>
-    <row r="10" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="10" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A10">
         <v>9</v>
       </c>
@@ -1150,7 +1144,7 @@
       </c>
       <c r="F10" s="26"/>
     </row>
-    <row r="11" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="11" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A11">
         <v>10</v>
       </c>
@@ -1166,7 +1160,7 @@
       </c>
       <c r="F11" s="26"/>
     </row>
-    <row r="12" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="12" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A12">
         <v>11</v>
       </c>
@@ -1182,7 +1176,7 @@
       </c>
       <c r="F12" s="26"/>
     </row>
-    <row r="13" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="13" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A13">
         <v>12</v>
       </c>
@@ -1198,7 +1192,7 @@
       </c>
       <c r="F13" s="26"/>
     </row>
-    <row r="14" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="14" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A14">
         <v>13</v>
       </c>
@@ -1214,7 +1208,7 @@
       </c>
       <c r="F14" s="26"/>
     </row>
-    <row r="15" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="15" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A15">
         <v>14</v>
       </c>
@@ -1230,7 +1224,7 @@
       </c>
       <c r="F15" s="26"/>
     </row>
-    <row r="16" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="16" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A16">
         <v>15</v>
       </c>
@@ -1246,7 +1240,7 @@
       </c>
       <c r="F16" s="26"/>
     </row>
-    <row r="17" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="17" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A17">
         <v>16</v>
       </c>
@@ -1262,7 +1256,7 @@
       </c>
       <c r="F17" s="26"/>
     </row>
-    <row r="18" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="18" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A18">
         <v>17</v>
       </c>
@@ -1278,7 +1272,7 @@
       </c>
       <c r="F18" s="26"/>
     </row>
-    <row r="19" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="19" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A19">
         <v>18</v>
       </c>
@@ -1294,7 +1288,7 @@
       </c>
       <c r="F19" s="26"/>
     </row>
-    <row r="20" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="20" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A20">
         <v>19</v>
       </c>
@@ -1310,7 +1304,7 @@
       </c>
       <c r="F20" s="26"/>
     </row>
-    <row r="21" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="21" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A21">
         <v>20</v>
       </c>
@@ -1326,7 +1320,7 @@
       </c>
       <c r="F21" s="26"/>
     </row>
-    <row r="22" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="22" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A22">
         <v>21</v>
       </c>
@@ -1342,7 +1336,7 @@
       </c>
       <c r="F22" s="26"/>
     </row>
-    <row r="23" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="23" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A23">
         <v>22</v>
       </c>
@@ -1358,7 +1352,7 @@
       </c>
       <c r="F23" s="26"/>
     </row>
-    <row r="24" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="24" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A24">
         <v>23</v>
       </c>
@@ -1374,7 +1368,7 @@
       </c>
       <c r="F24" s="26"/>
     </row>
-    <row r="25" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="25" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A25">
         <v>24</v>
       </c>
@@ -1390,7 +1384,7 @@
       </c>
       <c r="F25" s="26"/>
     </row>
-    <row r="26" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="26" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A26">
         <v>25</v>
       </c>
@@ -1406,7 +1400,7 @@
       </c>
       <c r="F26" s="26"/>
     </row>
-    <row r="27" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="27" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A27">
         <v>26</v>
       </c>
@@ -1422,7 +1416,7 @@
       </c>
       <c r="F27" s="26"/>
     </row>
-    <row r="28" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="28" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A28">
         <v>27</v>
       </c>
@@ -1438,7 +1432,7 @@
       </c>
       <c r="F28" s="26"/>
     </row>
-    <row r="29" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="29" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A29">
         <v>28</v>
       </c>
@@ -1454,7 +1448,7 @@
       </c>
       <c r="F29" s="26"/>
     </row>
-    <row r="30" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="30" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A30">
         <v>29</v>
       </c>
@@ -1470,7 +1464,7 @@
       </c>
       <c r="F30" s="26"/>
     </row>
-    <row r="31" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="31" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A31">
         <v>30</v>
       </c>
@@ -1486,7 +1480,7 @@
       </c>
       <c r="F31" s="26"/>
     </row>
-    <row r="32" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="32" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A32">
         <v>31</v>
       </c>
@@ -1502,7 +1496,7 @@
       </c>
       <c r="F32" s="26"/>
     </row>
-    <row r="33" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="33" spans="1:6" ht="27" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A33">
         <v>32</v>
       </c>
@@ -1518,7 +1512,7 @@
       </c>
       <c r="F33" s="26"/>
     </row>
-    <row r="34" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="34" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A34">
         <v>33</v>
       </c>
@@ -1534,7 +1528,7 @@
       </c>
       <c r="F34" s="26"/>
     </row>
-    <row r="35" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="35" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A35">
         <v>34</v>
       </c>
@@ -1550,7 +1544,7 @@
       </c>
       <c r="F35" s="26"/>
     </row>
-    <row r="36" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="36" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A36">
         <v>35</v>
       </c>
@@ -1566,7 +1560,7 @@
       </c>
       <c r="F36" s="26"/>
     </row>
-    <row r="37" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="37" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A37">
         <v>36</v>
       </c>
@@ -1582,7 +1576,7 @@
       </c>
       <c r="F37" s="26"/>
     </row>
-    <row r="38" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="38" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A38">
         <v>37</v>
       </c>
@@ -1598,7 +1592,7 @@
       </c>
       <c r="F38" s="26"/>
     </row>
-    <row r="39" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="39" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A39">
         <v>38</v>
       </c>
@@ -1614,7 +1608,7 @@
       </c>
       <c r="F39" s="26"/>
     </row>
-    <row r="40" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="40" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A40">
         <v>39</v>
       </c>
@@ -1630,7 +1624,7 @@
       </c>
       <c r="F40" s="26"/>
     </row>
-    <row r="41" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="41" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A41">
         <v>40</v>
       </c>
@@ -1646,7 +1640,7 @@
       </c>
       <c r="F41" s="26"/>
     </row>
-    <row r="42" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="42" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A42">
         <v>41</v>
       </c>
@@ -1662,7 +1656,7 @@
       </c>
       <c r="F42" s="26"/>
     </row>
-    <row r="43" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="43" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A43">
         <v>42</v>
       </c>
@@ -1678,7 +1672,7 @@
       </c>
       <c r="F43" s="26"/>
     </row>
-    <row r="44" spans="1:6" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="44" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A44" s="3">
         <f t="shared" ref="A44:A107" si="2">ROW() - 1</f>
         <v>43</v>
@@ -1692,7 +1686,7 @@
       <c r="E44" s="6"/>
       <c r="F44" s="7"/>
     </row>
-    <row r="45" spans="1:6" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="45" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A45" s="8">
         <f t="shared" si="2"/>
         <v>44</v>
@@ -1706,7 +1700,7 @@
       <c r="E45" s="11"/>
       <c r="F45" s="12"/>
     </row>
-    <row r="46" spans="1:6" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="46" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A46" s="3">
         <f t="shared" si="2"/>
         <v>45</v>
@@ -1720,7 +1714,7 @@
       <c r="E46" s="6"/>
       <c r="F46" s="7"/>
     </row>
-    <row r="47" spans="1:6" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="47" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A47" s="8">
         <f t="shared" si="2"/>
         <v>46</v>
@@ -1734,7 +1728,7 @@
       <c r="E47" s="11"/>
       <c r="F47" s="12"/>
     </row>
-    <row r="48" spans="1:6" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="48" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A48" s="3">
         <f t="shared" si="2"/>
         <v>47</v>
@@ -1748,7 +1742,7 @@
       <c r="E48" s="6"/>
       <c r="F48" s="7"/>
     </row>
-    <row r="49" spans="1:6" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="49" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A49" s="8">
         <f t="shared" si="2"/>
         <v>48</v>
@@ -1762,7 +1756,7 @@
       <c r="E49" s="11"/>
       <c r="F49" s="12"/>
     </row>
-    <row r="50" spans="1:6" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="50" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A50" s="3">
         <f t="shared" si="2"/>
         <v>49</v>
@@ -1776,7 +1770,7 @@
       <c r="E50" s="6"/>
       <c r="F50" s="7"/>
     </row>
-    <row r="51" spans="1:6" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="51" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A51" s="8">
         <f t="shared" si="2"/>
         <v>50</v>
@@ -1790,7 +1784,7 @@
       <c r="E51" s="11"/>
       <c r="F51" s="12"/>
     </row>
-    <row r="52" spans="1:6" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="52" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A52" s="3">
         <f t="shared" si="2"/>
         <v>51</v>
@@ -1804,7 +1798,7 @@
       <c r="E52" s="6"/>
       <c r="F52" s="7"/>
     </row>
-    <row r="53" spans="1:6" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="53" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A53" s="8">
         <f t="shared" si="2"/>
         <v>52</v>
@@ -1818,7 +1812,7 @@
       <c r="E53" s="11"/>
       <c r="F53" s="12"/>
     </row>
-    <row r="54" spans="1:6" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="54" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A54" s="3">
         <f t="shared" si="2"/>
         <v>53</v>
@@ -1832,7 +1826,7 @@
       <c r="E54" s="6"/>
       <c r="F54" s="7"/>
     </row>
-    <row r="55" spans="1:6" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="55" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A55" s="8">
         <f t="shared" si="2"/>
         <v>54</v>
@@ -1846,7 +1840,7 @@
       <c r="E55" s="11"/>
       <c r="F55" s="12"/>
     </row>
-    <row r="56" spans="1:6" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="56" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A56" s="3">
         <f t="shared" si="2"/>
         <v>55</v>
@@ -1860,7 +1854,7 @@
       <c r="E56" s="6"/>
       <c r="F56" s="7"/>
     </row>
-    <row r="57" spans="1:6" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="57" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A57" s="8">
         <f t="shared" si="2"/>
         <v>56</v>
@@ -1874,7 +1868,7 @@
       <c r="E57" s="11"/>
       <c r="F57" s="12"/>
     </row>
-    <row r="58" spans="1:6" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="58" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A58" s="3">
         <f t="shared" si="2"/>
         <v>57</v>
@@ -1888,7 +1882,7 @@
       <c r="E58" s="6"/>
       <c r="F58" s="7"/>
     </row>
-    <row r="59" spans="1:6" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="59" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A59" s="8">
         <f t="shared" si="2"/>
         <v>58</v>
@@ -1902,7 +1896,7 @@
       <c r="E59" s="11"/>
       <c r="F59" s="12"/>
     </row>
-    <row r="60" spans="1:6" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="60" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A60" s="3">
         <f t="shared" si="2"/>
         <v>59</v>
@@ -1916,7 +1910,7 @@
       <c r="E60" s="6"/>
       <c r="F60" s="7"/>
     </row>
-    <row r="61" spans="1:6" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="61" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A61" s="8">
         <f t="shared" si="2"/>
         <v>60</v>
@@ -1930,7 +1924,7 @@
       <c r="E61" s="11"/>
       <c r="F61" s="12"/>
     </row>
-    <row r="62" spans="1:6" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="62" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A62" s="3">
         <f t="shared" si="2"/>
         <v>61</v>
@@ -1944,7 +1938,7 @@
       <c r="E62" s="6"/>
       <c r="F62" s="7"/>
     </row>
-    <row r="63" spans="1:6" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="63" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A63" s="8">
         <f t="shared" si="2"/>
         <v>62</v>
@@ -1958,7 +1952,7 @@
       <c r="E63" s="11"/>
       <c r="F63" s="12"/>
     </row>
-    <row r="64" spans="1:6" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="64" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A64" s="3">
         <f t="shared" si="2"/>
         <v>63</v>
@@ -1972,7 +1966,7 @@
       <c r="E64" s="6"/>
       <c r="F64" s="7"/>
     </row>
-    <row r="65" spans="1:6" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="65" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A65" s="8">
         <f t="shared" si="2"/>
         <v>64</v>
@@ -1986,7 +1980,7 @@
       <c r="E65" s="11"/>
       <c r="F65" s="12"/>
     </row>
-    <row r="66" spans="1:6" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="66" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A66" s="3">
         <f t="shared" si="2"/>
         <v>65</v>
@@ -2000,7 +1994,7 @@
       <c r="E66" s="6"/>
       <c r="F66" s="7"/>
     </row>
-    <row r="67" spans="1:6" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="67" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A67" s="8">
         <f t="shared" si="2"/>
         <v>66</v>
@@ -2018,7 +2012,7 @@
       <c r="E67" s="11"/>
       <c r="F67" s="12"/>
     </row>
-    <row r="68" spans="1:6" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="68" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A68" s="3">
         <f t="shared" si="2"/>
         <v>67</v>
@@ -2036,7 +2030,7 @@
       <c r="E68" s="6"/>
       <c r="F68" s="7"/>
     </row>
-    <row r="69" spans="1:6" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="69" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A69" s="8">
         <f t="shared" si="2"/>
         <v>68</v>
@@ -2054,7 +2048,7 @@
       <c r="E69" s="11"/>
       <c r="F69" s="12"/>
     </row>
-    <row r="70" spans="1:6" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="70" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A70" s="3">
         <f t="shared" si="2"/>
         <v>69</v>
@@ -2072,7 +2066,7 @@
       <c r="E70" s="6"/>
       <c r="F70" s="7"/>
     </row>
-    <row r="71" spans="1:6" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="71" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A71" s="8">
         <f t="shared" si="2"/>
         <v>70</v>
@@ -2090,7 +2084,7 @@
       <c r="E71" s="11"/>
       <c r="F71" s="12"/>
     </row>
-    <row r="72" spans="1:6" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="72" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A72" s="3">
         <f t="shared" si="2"/>
         <v>71</v>
@@ -2108,7 +2102,7 @@
       <c r="E72" s="6"/>
       <c r="F72" s="7"/>
     </row>
-    <row r="73" spans="1:6" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="73" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A73" s="8">
         <f t="shared" si="2"/>
         <v>72</v>
@@ -2122,7 +2116,7 @@
       <c r="E73" s="11"/>
       <c r="F73" s="12"/>
     </row>
-    <row r="74" spans="1:6" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="74" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A74" s="3">
         <f t="shared" si="2"/>
         <v>73</v>
@@ -2140,7 +2134,7 @@
       <c r="E74" s="6"/>
       <c r="F74" s="7"/>
     </row>
-    <row r="75" spans="1:6" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="75" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A75" s="8">
         <f t="shared" si="2"/>
         <v>74</v>
@@ -2158,7 +2152,7 @@
       <c r="E75" s="11"/>
       <c r="F75" s="12"/>
     </row>
-    <row r="76" spans="1:6" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="76" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A76" s="3">
         <f t="shared" si="2"/>
         <v>75</v>
@@ -2176,7 +2170,7 @@
       <c r="E76" s="6"/>
       <c r="F76" s="7"/>
     </row>
-    <row r="77" spans="1:6" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="77" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A77" s="8">
         <f t="shared" si="2"/>
         <v>76</v>
@@ -2194,7 +2188,7 @@
       <c r="E77" s="11"/>
       <c r="F77" s="12"/>
     </row>
-    <row r="78" spans="1:6" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="78" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A78" s="3">
         <f t="shared" si="2"/>
         <v>77</v>
@@ -2212,7 +2206,7 @@
       <c r="E78" s="6"/>
       <c r="F78" s="7"/>
     </row>
-    <row r="79" spans="1:6" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="79" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A79" s="8">
         <f t="shared" si="2"/>
         <v>78</v>
@@ -2230,7 +2224,7 @@
       <c r="E79" s="11"/>
       <c r="F79" s="12"/>
     </row>
-    <row r="80" spans="1:6" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="80" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A80" s="3">
         <f t="shared" si="2"/>
         <v>79</v>
@@ -2248,7 +2242,7 @@
       <c r="E80" s="6"/>
       <c r="F80" s="7"/>
     </row>
-    <row r="81" spans="1:6" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="81" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A81" s="8">
         <f t="shared" si="2"/>
         <v>80</v>
@@ -2266,7 +2260,7 @@
       <c r="E81" s="11"/>
       <c r="F81" s="12"/>
     </row>
-    <row r="82" spans="1:6" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="82" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A82" s="3">
         <f t="shared" si="2"/>
         <v>81</v>
@@ -2284,7 +2278,7 @@
       <c r="E82" s="6"/>
       <c r="F82" s="7"/>
     </row>
-    <row r="83" spans="1:6" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="83" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A83" s="8">
         <f t="shared" si="2"/>
         <v>82</v>
@@ -2302,7 +2296,7 @@
       <c r="E83" s="11"/>
       <c r="F83" s="12"/>
     </row>
-    <row r="84" spans="1:6" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="84" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A84" s="3">
         <f t="shared" si="2"/>
         <v>83</v>
@@ -2320,7 +2314,7 @@
       <c r="E84" s="6"/>
       <c r="F84" s="7"/>
     </row>
-    <row r="85" spans="1:6" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="85" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A85" s="8">
         <f t="shared" si="2"/>
         <v>84</v>
@@ -2338,7 +2332,7 @@
       <c r="E85" s="11"/>
       <c r="F85" s="12"/>
     </row>
-    <row r="86" spans="1:6" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="86" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A86" s="3">
         <f t="shared" si="2"/>
         <v>85</v>
@@ -2356,7 +2350,7 @@
       <c r="E86" s="6"/>
       <c r="F86" s="7"/>
     </row>
-    <row r="87" spans="1:6" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="87" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A87" s="8">
         <f t="shared" si="2"/>
         <v>86</v>
@@ -2374,7 +2368,7 @@
       <c r="E87" s="11"/>
       <c r="F87" s="12"/>
     </row>
-    <row r="88" spans="1:6" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="88" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A88" s="3">
         <f t="shared" si="2"/>
         <v>87</v>
@@ -2392,7 +2386,7 @@
       <c r="E88" s="6"/>
       <c r="F88" s="7"/>
     </row>
-    <row r="89" spans="1:6" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="89" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A89" s="8">
         <f t="shared" si="2"/>
         <v>88</v>
@@ -2410,7 +2404,7 @@
       <c r="E89" s="11"/>
       <c r="F89" s="12"/>
     </row>
-    <row r="90" spans="1:6" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="90" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A90" s="3">
         <f t="shared" si="2"/>
         <v>89</v>
@@ -2428,7 +2422,7 @@
       <c r="E90" s="6"/>
       <c r="F90" s="7"/>
     </row>
-    <row r="91" spans="1:6" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="91" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A91" s="8">
         <f t="shared" si="2"/>
         <v>90</v>
@@ -2442,7 +2436,7 @@
       <c r="E91" s="11"/>
       <c r="F91" s="12"/>
     </row>
-    <row r="92" spans="1:6" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="92" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A92" s="3">
         <f t="shared" si="2"/>
         <v>91</v>
@@ -2456,7 +2450,7 @@
       <c r="E92" s="6"/>
       <c r="F92" s="7"/>
     </row>
-    <row r="93" spans="1:6" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="93" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A93" s="8">
         <f t="shared" si="2"/>
         <v>92</v>
@@ -2470,7 +2464,7 @@
       <c r="E93" s="11"/>
       <c r="F93" s="12"/>
     </row>
-    <row r="94" spans="1:6" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="94" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A94" s="3">
         <f t="shared" si="2"/>
         <v>93</v>
@@ -2484,7 +2478,7 @@
       <c r="E94" s="6"/>
       <c r="F94" s="7"/>
     </row>
-    <row r="95" spans="1:6" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="95" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A95" s="8">
         <f t="shared" si="2"/>
         <v>94</v>
@@ -2498,7 +2492,7 @@
       <c r="E95" s="11"/>
       <c r="F95" s="12"/>
     </row>
-    <row r="96" spans="1:6" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="96" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A96" s="3">
         <f t="shared" si="2"/>
         <v>95</v>
@@ -2512,7 +2506,7 @@
       <c r="E96" s="6"/>
       <c r="F96" s="7"/>
     </row>
-    <row r="97" spans="1:6" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="97" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A97" s="8">
         <f t="shared" si="2"/>
         <v>96</v>
@@ -2526,7 +2520,7 @@
       <c r="E97" s="11"/>
       <c r="F97" s="12"/>
     </row>
-    <row r="98" spans="1:6" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="98" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A98" s="3">
         <f t="shared" si="2"/>
         <v>97</v>
@@ -2540,7 +2534,7 @@
       <c r="E98" s="6"/>
       <c r="F98" s="7"/>
     </row>
-    <row r="99" spans="1:6" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="99" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A99" s="8">
         <f t="shared" si="2"/>
         <v>98</v>
@@ -2554,7 +2548,7 @@
       <c r="E99" s="11"/>
       <c r="F99" s="12"/>
     </row>
-    <row r="100" spans="1:6" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="100" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A100" s="3">
         <f t="shared" si="2"/>
         <v>99</v>
@@ -2568,7 +2562,7 @@
       <c r="E100" s="6"/>
       <c r="F100" s="7"/>
     </row>
-    <row r="101" spans="1:6" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="101" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A101" s="8">
         <f t="shared" si="2"/>
         <v>100</v>
@@ -2582,7 +2576,7 @@
       <c r="E101" s="11"/>
       <c r="F101" s="12"/>
     </row>
-    <row r="102" spans="1:6" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="102" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A102" s="3">
         <f t="shared" si="2"/>
         <v>101</v>
@@ -2596,7 +2590,7 @@
       <c r="E102" s="6"/>
       <c r="F102" s="7"/>
     </row>
-    <row r="103" spans="1:6" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="103" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A103" s="8">
         <f t="shared" si="2"/>
         <v>102</v>
@@ -2610,7 +2604,7 @@
       <c r="E103" s="11"/>
       <c r="F103" s="12"/>
     </row>
-    <row r="104" spans="1:6" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="104" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A104" s="3">
         <f t="shared" si="2"/>
         <v>103</v>
@@ -2624,7 +2618,7 @@
       <c r="E104" s="6"/>
       <c r="F104" s="7"/>
     </row>
-    <row r="105" spans="1:6" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="105" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A105" s="8">
         <f t="shared" si="2"/>
         <v>104</v>
@@ -2638,7 +2632,7 @@
       <c r="E105" s="11"/>
       <c r="F105" s="12"/>
     </row>
-    <row r="106" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="106" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A106" s="3">
         <f t="shared" si="2"/>
         <v>105</v>
@@ -2652,7 +2646,7 @@
       <c r="E106" s="6"/>
       <c r="F106" s="7"/>
     </row>
-    <row r="107" spans="1:6" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="107" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A107" s="8">
         <f t="shared" si="2"/>
         <v>106</v>
@@ -2666,7 +2660,7 @@
       <c r="E107" s="11"/>
       <c r="F107" s="12"/>
     </row>
-    <row r="108" spans="1:6" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="108" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A108" s="3">
         <f t="shared" ref="A108:A153" si="4">ROW() - 1</f>
         <v>107</v>
@@ -2680,7 +2674,7 @@
       <c r="E108" s="6"/>
       <c r="F108" s="7"/>
     </row>
-    <row r="109" spans="1:6" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="109" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A109" s="8">
         <f t="shared" si="4"/>
         <v>108</v>
@@ -2694,7 +2688,7 @@
       <c r="E109" s="11"/>
       <c r="F109" s="12"/>
     </row>
-    <row r="110" spans="1:6" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="110" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A110" s="3">
         <f t="shared" si="4"/>
         <v>109</v>
@@ -2708,7 +2702,7 @@
       <c r="E110" s="6"/>
       <c r="F110" s="7"/>
     </row>
-    <row r="111" spans="1:6" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="111" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A111" s="8">
         <f t="shared" si="4"/>
         <v>110</v>
@@ -2722,7 +2716,7 @@
       <c r="E111" s="11"/>
       <c r="F111" s="12"/>
     </row>
-    <row r="112" spans="1:6" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="112" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A112" s="3">
         <f t="shared" si="4"/>
         <v>111</v>
@@ -2736,7 +2730,7 @@
       <c r="E112" s="6"/>
       <c r="F112" s="7"/>
     </row>
-    <row r="113" spans="1:6" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="113" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A113" s="8">
         <f t="shared" si="4"/>
         <v>112</v>
@@ -2750,7 +2744,7 @@
       <c r="E113" s="11"/>
       <c r="F113" s="12"/>
     </row>
-    <row r="114" spans="1:6" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="114" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A114" s="3">
         <f t="shared" si="4"/>
         <v>113</v>
@@ -2764,7 +2758,7 @@
       <c r="E114" s="6"/>
       <c r="F114" s="7"/>
     </row>
-    <row r="115" spans="1:6" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="115" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A115" s="8">
         <f t="shared" si="4"/>
         <v>114</v>
@@ -2778,7 +2772,7 @@
       <c r="E115" s="11"/>
       <c r="F115" s="12"/>
     </row>
-    <row r="116" spans="1:6" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="116" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A116" s="3">
         <f t="shared" si="4"/>
         <v>115</v>
@@ -2792,7 +2786,7 @@
       <c r="E116" s="6"/>
       <c r="F116" s="7"/>
     </row>
-    <row r="117" spans="1:6" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="117" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A117" s="8">
         <f t="shared" si="4"/>
         <v>116</v>
@@ -2806,7 +2800,7 @@
       <c r="E117" s="11"/>
       <c r="F117" s="12"/>
     </row>
-    <row r="118" spans="1:6" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="118" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A118" s="3">
         <f t="shared" si="4"/>
         <v>117</v>
@@ -2820,7 +2814,7 @@
       <c r="E118" s="6"/>
       <c r="F118" s="7"/>
     </row>
-    <row r="119" spans="1:6" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="119" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A119" s="8">
         <f t="shared" si="4"/>
         <v>118</v>
@@ -2834,7 +2828,7 @@
       <c r="E119" s="11"/>
       <c r="F119" s="12"/>
     </row>
-    <row r="120" spans="1:6" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="120" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A120" s="3">
         <f t="shared" si="4"/>
         <v>119</v>
@@ -2848,7 +2842,7 @@
       <c r="E120" s="6"/>
       <c r="F120" s="7"/>
     </row>
-    <row r="121" spans="1:6" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="121" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A121" s="8">
         <f t="shared" si="4"/>
         <v>120</v>
@@ -2862,7 +2856,7 @@
       <c r="E121" s="11"/>
       <c r="F121" s="12"/>
     </row>
-    <row r="122" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="122" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A122" s="3">
         <f t="shared" si="4"/>
         <v>121</v>
@@ -2876,7 +2870,7 @@
       <c r="E122" s="6"/>
       <c r="F122" s="7"/>
     </row>
-    <row r="123" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="123" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A123" s="8">
         <f t="shared" si="4"/>
         <v>122</v>
@@ -2890,7 +2884,7 @@
       <c r="E123" s="11"/>
       <c r="F123" s="12"/>
     </row>
-    <row r="124" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="124" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A124" s="3">
         <f t="shared" si="4"/>
         <v>123</v>
@@ -2904,7 +2898,7 @@
       <c r="E124" s="6"/>
       <c r="F124" s="7"/>
     </row>
-    <row r="125" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="125" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A125" s="8">
         <f t="shared" si="4"/>
         <v>124</v>
@@ -2918,7 +2912,7 @@
       <c r="E125" s="11"/>
       <c r="F125" s="12"/>
     </row>
-    <row r="126" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="126" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A126" s="3">
         <f t="shared" si="4"/>
         <v>125</v>
@@ -2932,7 +2926,7 @@
       <c r="E126" s="6"/>
       <c r="F126" s="7"/>
     </row>
-    <row r="127" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="127" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A127" s="8">
         <f t="shared" si="4"/>
         <v>126</v>
@@ -2946,7 +2940,7 @@
       <c r="E127" s="11"/>
       <c r="F127" s="12"/>
     </row>
-    <row r="128" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="128" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A128" s="3">
         <f t="shared" si="4"/>
         <v>127</v>
@@ -2960,7 +2954,7 @@
       <c r="E128" s="6"/>
       <c r="F128" s="7"/>
     </row>
-    <row r="129" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="129" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A129" s="8">
         <f t="shared" si="4"/>
         <v>128</v>
@@ -2974,7 +2968,7 @@
       <c r="E129" s="11"/>
       <c r="F129" s="12"/>
     </row>
-    <row r="130" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="130" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A130" s="3">
         <f t="shared" si="4"/>
         <v>129</v>
@@ -2988,7 +2982,7 @@
       <c r="E130" s="6"/>
       <c r="F130" s="7"/>
     </row>
-    <row r="131" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="131" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A131" s="8">
         <f t="shared" si="4"/>
         <v>130</v>
@@ -3002,7 +2996,7 @@
       <c r="E131" s="11"/>
       <c r="F131" s="12"/>
     </row>
-    <row r="132" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="132" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A132" s="3">
         <f t="shared" si="4"/>
         <v>131</v>
@@ -3016,7 +3010,7 @@
       <c r="E132" s="6"/>
       <c r="F132" s="7"/>
     </row>
-    <row r="133" spans="1:6" ht="17" thickBot="1" x14ac:dyDescent="0.5">
+    <row r="133" spans="1:6" ht="18" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A133" s="8">
         <f t="shared" si="4"/>
         <v>132</v>
@@ -3030,7 +3024,7 @@
       <c r="E133" s="11"/>
       <c r="F133" s="12"/>
     </row>
-    <row r="134" spans="1:6" ht="17" thickBot="1" x14ac:dyDescent="0.5">
+    <row r="134" spans="1:6" ht="18" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A134" s="3">
         <f t="shared" si="4"/>
         <v>133</v>
@@ -3044,7 +3038,7 @@
       <c r="E134" s="6"/>
       <c r="F134" s="7"/>
     </row>
-    <row r="135" spans="1:6" ht="15.5" thickBot="1" x14ac:dyDescent="0.45">
+    <row r="135" spans="1:6" ht="17.25" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A135" s="8">
         <f t="shared" si="4"/>
         <v>134</v>
@@ -3058,7 +3052,7 @@
       <c r="E135" s="11"/>
       <c r="F135" s="12"/>
     </row>
-    <row r="136" spans="1:6" ht="15.5" thickBot="1" x14ac:dyDescent="0.45">
+    <row r="136" spans="1:6" ht="17.25" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A136" s="3">
         <f t="shared" si="4"/>
         <v>135</v>
@@ -3072,7 +3066,7 @@
       <c r="E136" s="6"/>
       <c r="F136" s="7"/>
     </row>
-    <row r="137" spans="1:6" ht="15.5" thickBot="1" x14ac:dyDescent="0.45">
+    <row r="137" spans="1:6" ht="17.25" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A137" s="8">
         <f t="shared" si="4"/>
         <v>136</v>
@@ -3086,7 +3080,7 @@
       <c r="E137" s="11"/>
       <c r="F137" s="12"/>
     </row>
-    <row r="138" spans="1:6" ht="15.5" thickBot="1" x14ac:dyDescent="0.45">
+    <row r="138" spans="1:6" ht="17.25" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A138" s="3">
         <f t="shared" si="4"/>
         <v>137</v>
@@ -3100,7 +3094,7 @@
       <c r="E138" s="6"/>
       <c r="F138" s="7"/>
     </row>
-    <row r="139" spans="1:6" ht="15.5" thickBot="1" x14ac:dyDescent="0.45">
+    <row r="139" spans="1:6" ht="17.25" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A139" s="8">
         <f t="shared" si="4"/>
         <v>138</v>
@@ -3114,7 +3108,7 @@
       <c r="E139" s="11"/>
       <c r="F139" s="12"/>
     </row>
-    <row r="140" spans="1:6" ht="15.5" thickBot="1" x14ac:dyDescent="0.45">
+    <row r="140" spans="1:6" ht="17.25" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A140" s="3">
         <f t="shared" si="4"/>
         <v>139</v>
@@ -3128,7 +3122,7 @@
       <c r="E140" s="6"/>
       <c r="F140" s="7"/>
     </row>
-    <row r="141" spans="1:6" ht="15.5" thickBot="1" x14ac:dyDescent="0.45">
+    <row r="141" spans="1:6" ht="17.25" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A141" s="8">
         <f t="shared" si="4"/>
         <v>140</v>
@@ -3142,7 +3136,7 @@
       <c r="E141" s="11"/>
       <c r="F141" s="12"/>
     </row>
-    <row r="142" spans="1:6" ht="15.5" thickBot="1" x14ac:dyDescent="0.45">
+    <row r="142" spans="1:6" ht="17.25" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A142" s="3">
         <f t="shared" si="4"/>
         <v>141</v>
@@ -3156,7 +3150,7 @@
       <c r="E142" s="6"/>
       <c r="F142" s="7"/>
     </row>
-    <row r="143" spans="1:6" ht="15" x14ac:dyDescent="0.4">
+    <row r="143" spans="1:6" ht="16.5" x14ac:dyDescent="0.35">
       <c r="A143" s="8">
         <f t="shared" si="4"/>
         <v>142</v>
@@ -3170,7 +3164,7 @@
       <c r="E143" s="11"/>
       <c r="F143" s="12"/>
     </row>
-    <row r="144" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="144" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A144" s="3">
         <f t="shared" si="4"/>
         <v>143</v>
@@ -3184,7 +3178,7 @@
       <c r="E144" s="6"/>
       <c r="F144" s="7"/>
     </row>
-    <row r="145" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="145" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A145" s="8">
         <f t="shared" si="4"/>
         <v>144</v>
@@ -3198,7 +3192,7 @@
       <c r="E145" s="11"/>
       <c r="F145" s="12"/>
     </row>
-    <row r="146" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="146" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A146" s="3">
         <f t="shared" si="4"/>
         <v>145</v>
@@ -3212,7 +3206,7 @@
       <c r="E146" s="6"/>
       <c r="F146" s="7"/>
     </row>
-    <row r="147" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="147" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A147" s="8">
         <f t="shared" si="4"/>
         <v>146</v>
@@ -3226,7 +3220,7 @@
       <c r="E147" s="11"/>
       <c r="F147" s="12"/>
     </row>
-    <row r="148" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="148" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A148" s="3">
         <f t="shared" si="4"/>
         <v>147</v>
@@ -3240,7 +3234,7 @@
       <c r="E148" s="6"/>
       <c r="F148" s="7"/>
     </row>
-    <row r="149" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="149" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A149" s="8">
         <f t="shared" si="4"/>
         <v>148</v>
@@ -3254,7 +3248,7 @@
       <c r="E149" s="11"/>
       <c r="F149" s="12"/>
     </row>
-    <row r="150" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="150" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A150" s="3">
         <f t="shared" si="4"/>
         <v>149</v>
@@ -3268,7 +3262,7 @@
       <c r="E150" s="6"/>
       <c r="F150" s="7"/>
     </row>
-    <row r="151" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="151" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A151" s="8">
         <f t="shared" si="4"/>
         <v>150</v>
@@ -3282,7 +3276,7 @@
       <c r="E151" s="11"/>
       <c r="F151" s="12"/>
     </row>
-    <row r="152" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="152" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A152" s="3">
         <f t="shared" si="4"/>
         <v>151</v>
@@ -3296,7 +3290,7 @@
       <c r="E152" s="6"/>
       <c r="F152" s="7"/>
     </row>
-    <row r="153" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="153" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A153" s="8">
         <f t="shared" si="4"/>
         <v>152</v>
@@ -3310,7 +3304,7 @@
       <c r="E153" s="11"/>
       <c r="F153" s="12"/>
     </row>
-    <row r="154" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="154" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A154" s="3">
         <f>ROW() - 1</f>
         <v>153</v>
@@ -3324,7 +3318,7 @@
       <c r="E154" s="6"/>
       <c r="F154" s="7"/>
     </row>
-    <row r="155" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="155" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A155" s="8">
         <v>154</v>
       </c>

</xml_diff>